<commit_message>
Deploying to gh-pages from @ Alvearie/alvearie-fhir-ig@01171653529c30e87fa8f00be76c3b3fad2e30d8 🚀
</commit_message>
<xml_diff>
--- a/2.0.0/StructureDefinition-cdm-organization-affiliation.xlsx
+++ b/2.0.0/StructureDefinition-cdm-organization-affiliation.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2021-09-28T19:40:31+00:00</t>
+    <t>2021-10-01T15:07:10+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -718,7 +718,7 @@
     <t>SourceClassificationTag</t>
   </si>
   <si>
-    <t>Identifies the origin of data elements in this FHIR resource, from either primary or secondary source systems</t>
+    <t>Identifies the origin of this FHIR resource, from either a source system of record or derived from a process</t>
   </si>
   <si>
     <t>OrganizationAffiliation.meta.tag.id</t>
@@ -742,7 +742,7 @@
     <t>Need to be unambiguous about the source of the definition of the symbol.</t>
   </si>
   <si>
-    <t>http://ibm.com/fhir/cdm/CodeSystem/process-meta-primary-or-secondary</t>
+    <t>http://ibm.com/fhir/cdm/CodeSystem/process-meta-source-classification</t>
   </si>
   <si>
     <t>Coding.system</t>

</xml_diff>